<commit_message>
Added all tagging and file download functionality
</commit_message>
<xml_diff>
--- a/files/myfile.xlsx
+++ b/files/myfile.xlsx
@@ -2,12 +2,12 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
-  <workbookProtection/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="tags" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -17,10 +17,18 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <b val="1"/>
       <color theme="1"/>
       <sz val="11"/>
       <scheme val="minor"/>
@@ -37,12 +45,27 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -55,14 +78,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
@@ -427,6 +453,74 @@
   </sheetPr>
   <dimension ref="A1:A7"/>
   <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Statement</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>The rooms were bad but staff was friendly.</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Weather is good but it smells .</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>It is hot but scenery is good .</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Laptop is fast but it's heavy .</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Phone is fast but battery is very less .</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>The rooms were clean but staff was rude .</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:C5"/>
+  <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
@@ -434,9 +528,19 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="inlineStr">
+      <c r="A1" s="2" t="inlineStr">
         <is>
           <t>Statement</t>
+        </is>
+      </c>
+      <c r="B1" s="2" t="inlineStr">
+        <is>
+          <t>Aspect</t>
+        </is>
+      </c>
+      <c r="C1" s="2" t="inlineStr">
+        <is>
+          <t>Sentiment</t>
         </is>
       </c>
     </row>
@@ -446,11 +550,31 @@
           <t>The rooms were bad but staff was friendly.</t>
         </is>
       </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>room</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>NEG</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Weather is good but it smells .</t>
+          <t>It is hot but scenery is good .</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>weather</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>NEG</t>
         </is>
       </c>
     </row>
@@ -460,25 +584,31 @@
           <t>It is hot but scenery is good .</t>
         </is>
       </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>scenery</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>POS</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Laptop is fast but it's heavy .</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>Phone is fast but battery is very less .</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>The rooms were clean but staff was rude .</t>
+          <t>The rooms were bad but staff was friendly.</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>staff</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>POS</t>
         </is>
       </c>
     </row>

</xml_diff>